<commit_message>
push exp results for thesis topic1
</commit_message>
<xml_diff>
--- a/output/experiments/thesis_topic1/6h-bat-12months-0.6dc.xlsx
+++ b/output/experiments/thesis_topic1/6h-bat-12months-0.6dc.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="157">
   <si>
     <t>status</t>
   </si>
@@ -416,6 +416,75 @@
   </si>
   <si>
     <t>MPC-MPC-optimal-GT-unconscious-1.5-0.6-0.6-flex-438-unconscious-09-01-10-01-Sum-ALL-Sum-nan-nan-2023-08-28_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-Prediction-unconscious-1.5-0.6-0.6-flex-438-unconscious-09-01-10-01-Sum-ALL-Sum-nan-nan-2023-08-28_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-Disturbance-unconscious-1.5-0.6-0.6-unif-438-unconscious-09-01-10-01-Sum-ALL-Sum-normal-0.03-2023-08-28_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-09-01-10-01-Sum-ALL-Sum-nan-nan-2023-08-28_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-Naive-unconscious-1.5-0.6-0.6-flex-438-unconscious-09-01-10-01-Sum-ALL-Sum-nan-nan-2023-08-28_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-RBC-MSC-GT-unconscious-1.5-0.6-0.6-unif-438-unconscious-09-01-10-01-Sum-ALL-Sum-nan-nan-2023-08-28_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-GT-unconscious-1.5-0.6-0.6-flex-438-unconscious-10-01-11-01-Sum-ALL-Sum-nan-nan-2023-08-28_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-Prediction-unconscious-1.5-0.6-0.6-flex-438-unconscious-10-01-11-01-Sum-ALL-Sum-nan-nan-2023-08-28_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-Disturbance-unconscious-1.5-0.6-0.6-unif-438-unconscious-10-01-11-01-Sum-ALL-Sum-normal-0.03-2023-08-28_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-10-01-11-01-Sum-ALL-Sum-nan-nan-2023-08-28_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-Naive-unconscious-1.5-0.6-0.6-flex-438-unconscious-10-01-11-01-Sum-ALL-Sum-nan-nan-2023-08-28_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-RBC-MSC-GT-unconscious-1.5-0.6-0.6-unif-438-unconscious-10-01-11-01-Sum-ALL-Sum-nan-nan-2023-08-28_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-GT-unconscious-1.5-0.6-0.6-flex-438-unconscious-11-01-12-01-Sum-ALL-Sum-nan-nan-2023-08-28_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-Prediction-unconscious-1.5-0.6-0.6-flex-438-unconscious-11-01-12-01-Sum-ALL-Sum-nan-nan-2023-08-28_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-Disturbance-unconscious-1.5-0.6-0.6-unif-438-unconscious-11-01-12-01-Sum-ALL-Sum-normal-0.03-2023-08-28_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-11-01-12-01-Sum-ALL-Sum-nan-nan-2023-08-28_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-Naive-unconscious-1.5-0.6-0.6-flex-438-unconscious-11-01-12-01-Sum-ALL-Sum-nan-nan-2023-08-28_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-RBC-MSC-GT-unconscious-1.5-0.6-0.6-unif-438-unconscious-11-01-12-01-Sum-ALL-Sum-nan-nan-2023-08-28_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-GT-unconscious-1.5-0.6-0.6-flex-438-unconscious-12-01-12-31-Sum-ALL-Sum-nan-nan-2023-08-28_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-Prediction-unconscious-1.5-0.6-0.6-flex-438-unconscious-12-01-12-31-Sum-ALL-Sum-nan-nan-2023-08-28_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-Disturbance-unconscious-1.5-0.6-0.6-unif-438-unconscious-12-01-12-31-Sum-ALL-Sum-normal-0.03-2023-08-28_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-Simple-unconscious-1.5-0.6-0.6-flex-438-unconscious-12-01-12-31-Sum-ALL-Sum-nan-nan-2023-08-28_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-MPC-optimal-Naive-unconscious-1.5-0.6-0.6-flex-438-unconscious-12-01-12-31-Sum-ALL-Sum-nan-nan-2023-08-28_001.xlsx</t>
+  </si>
+  <si>
+    <t>MPC-RBC-MSC-GT-unconscious-1.5-0.6-0.6-unif-438-unconscious-12-01-12-31-Sum-ALL-Sum-nan-nan-2023-08-28_001.xlsx</t>
   </si>
 </sst>
 </file>
@@ -7370,7 +7439,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C45" t="s">
         <v>57</v>
@@ -7420,8 +7489,104 @@
       <c r="R45" t="s">
         <v>82</v>
       </c>
+      <c r="U45">
+        <v>259.9689304420941</v>
+      </c>
+      <c r="V45">
+        <v>30.98958333333333</v>
+      </c>
+      <c r="W45">
+        <v>3913.832762100003</v>
+      </c>
       <c r="X45" t="s">
         <v>128</v>
+      </c>
+      <c r="Y45">
+        <v>259.9689304420941</v>
+      </c>
+      <c r="Z45">
+        <v>241.9689304420941</v>
+      </c>
+      <c r="AA45">
+        <v>18</v>
+      </c>
+      <c r="AB45">
+        <v>18</v>
+      </c>
+      <c r="AC45">
+        <v>438</v>
+      </c>
+      <c r="AD45">
+        <v>6.506139241770216</v>
+      </c>
+      <c r="AE45">
+        <v>0</v>
+      </c>
+      <c r="AF45">
+        <v>0</v>
+      </c>
+      <c r="AG45">
+        <v>0.1211411684798102</v>
+      </c>
+      <c r="AH45">
+        <v>0.1211411684798102</v>
+      </c>
+      <c r="AI45">
+        <v>0.1127534698847187</v>
+      </c>
+      <c r="AK45">
+        <v>105.72771822</v>
+      </c>
+      <c r="AL45">
+        <v>136.2412122220941</v>
+      </c>
+      <c r="AN45">
+        <v>54.59899159663865</v>
+      </c>
+      <c r="AO45">
+        <v>1615.704738151263</v>
+      </c>
+      <c r="AP45">
+        <v>530.2951205625114</v>
+      </c>
+      <c r="AQ45">
+        <v>2145.999858713774</v>
+      </c>
+      <c r="AR45">
+        <v>1110.784748030245</v>
+      </c>
+      <c r="AS45">
+        <v>1138.963731327242</v>
+      </c>
+      <c r="AT45">
+        <v>77.95116703029737</v>
+      </c>
+      <c r="AU45">
+        <v>148.4422916368418</v>
+      </c>
+      <c r="AV45">
+        <v>12.20107941474768</v>
+      </c>
+      <c r="AW45">
+        <v>176.2128637</v>
+      </c>
+      <c r="AX45">
+        <v>3.552713678800501E-15</v>
+      </c>
+      <c r="AY45">
+        <v>6.023539463669574E-16</v>
+      </c>
+      <c r="AZ45">
+        <v>-8.928770399999998</v>
+      </c>
+      <c r="BA45">
+        <v>7.429690699999995</v>
+      </c>
+      <c r="BB45">
+        <v>0</v>
+      </c>
+      <c r="BC45">
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:55">
@@ -7429,7 +7594,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C46" t="s">
         <v>57</v>
@@ -7485,8 +7650,104 @@
       <c r="T46">
         <v>0.03</v>
       </c>
+      <c r="U46">
+        <v>262.3256190672621</v>
+      </c>
+      <c r="V46">
+        <v>30.98958333333333</v>
+      </c>
+      <c r="W46">
+        <v>4008.1411921</v>
+      </c>
       <c r="X46" t="s">
         <v>129</v>
+      </c>
+      <c r="Y46">
+        <v>262.3256190672621</v>
+      </c>
+      <c r="Z46">
+        <v>244.3256190672621</v>
+      </c>
+      <c r="AA46">
+        <v>18</v>
+      </c>
+      <c r="AB46">
+        <v>18</v>
+      </c>
+      <c r="AC46">
+        <v>438</v>
+      </c>
+      <c r="AD46">
+        <v>6.506139241770216</v>
+      </c>
+      <c r="AE46">
+        <v>0</v>
+      </c>
+      <c r="AF46">
+        <v>0</v>
+      </c>
+      <c r="AG46">
+        <v>0.1222393459170541</v>
+      </c>
+      <c r="AH46">
+        <v>0.1222393459170541</v>
+      </c>
+      <c r="AI46">
+        <v>0.1138516473219627</v>
+      </c>
+      <c r="AK46">
+        <v>105.6205314550717</v>
+      </c>
+      <c r="AL46">
+        <v>138.7050876121904</v>
+      </c>
+      <c r="AN46">
+        <v>54.59899159663865</v>
+      </c>
+      <c r="AO46">
+        <v>1615.704738151263</v>
+      </c>
+      <c r="AP46">
+        <v>530.2951205625097</v>
+      </c>
+      <c r="AQ46">
+        <v>2145.999858713772</v>
+      </c>
+      <c r="AR46">
+        <v>1110.784748030245</v>
+      </c>
+      <c r="AS46">
+        <v>1121.067246091515</v>
+      </c>
+      <c r="AT46">
+        <v>59.30216006591483</v>
+      </c>
+      <c r="AU46">
+        <v>147.6309738583993</v>
+      </c>
+      <c r="AV46">
+        <v>8.925886246208846</v>
+      </c>
+      <c r="AW46">
+        <v>176.0342190917861</v>
+      </c>
+      <c r="AX46">
+        <v>2.220446049250313E-16</v>
+      </c>
+      <c r="AY46">
+        <v>3.764712164793484E-17</v>
+      </c>
+      <c r="AZ46">
+        <v>-9.027763313279181</v>
+      </c>
+      <c r="BA46">
+        <v>11.32321040387404</v>
+      </c>
+      <c r="BB46">
+        <v>0</v>
+      </c>
+      <c r="BC46">
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:55">
@@ -7494,7 +7755,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C47" t="s">
         <v>57</v>
@@ -7544,8 +7805,104 @@
       <c r="R47" t="s">
         <v>82</v>
       </c>
+      <c r="U47">
+        <v>258.413835312995</v>
+      </c>
+      <c r="V47">
+        <v>30.98958333333333</v>
+      </c>
+      <c r="W47">
+        <v>3434.058429600002</v>
+      </c>
       <c r="X47" t="s">
         <v>130</v>
+      </c>
+      <c r="Y47">
+        <v>258.413835312995</v>
+      </c>
+      <c r="Z47">
+        <v>240.413835312995</v>
+      </c>
+      <c r="AA47">
+        <v>18</v>
+      </c>
+      <c r="AB47">
+        <v>18</v>
+      </c>
+      <c r="AC47">
+        <v>438</v>
+      </c>
+      <c r="AD47">
+        <v>6.506139241770216</v>
+      </c>
+      <c r="AE47">
+        <v>0</v>
+      </c>
+      <c r="AF47">
+        <v>0</v>
+      </c>
+      <c r="AG47">
+        <v>0.1204165201892781</v>
+      </c>
+      <c r="AH47">
+        <v>0.1204165201892781</v>
+      </c>
+      <c r="AI47">
+        <v>0.1120288215941866</v>
+      </c>
+      <c r="AK47">
+        <v>104.352103293657</v>
+      </c>
+      <c r="AL47">
+        <v>136.0617320193381</v>
+      </c>
+      <c r="AN47">
+        <v>54.59899159663865</v>
+      </c>
+      <c r="AO47">
+        <v>1615.704738151263</v>
+      </c>
+      <c r="AP47">
+        <v>530.2951205625109</v>
+      </c>
+      <c r="AQ47">
+        <v>2145.999858713773</v>
+      </c>
+      <c r="AR47">
+        <v>1110.784748030245</v>
+      </c>
+      <c r="AS47">
+        <v>1141.184065907116</v>
+      </c>
+      <c r="AT47">
+        <v>79.87912893561716</v>
+      </c>
+      <c r="AU47">
+        <v>148.8232643084481</v>
+      </c>
+      <c r="AV47">
+        <v>12.76153228911005</v>
+      </c>
+      <c r="AW47">
+        <v>173.920172156095</v>
+      </c>
+      <c r="AX47">
+        <v>1.4210854715202E-14</v>
+      </c>
+      <c r="AY47">
+        <v>2.40941578546783E-15</v>
+      </c>
+      <c r="AZ47">
+        <v>-9.013058559235162</v>
+      </c>
+      <c r="BA47">
+        <v>11.60523589830271</v>
+      </c>
+      <c r="BB47">
+        <v>0</v>
+      </c>
+      <c r="BC47">
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:55">
@@ -7553,7 +7910,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C48" t="s">
         <v>57</v>
@@ -7603,16 +7960,112 @@
       <c r="R48" t="s">
         <v>82</v>
       </c>
+      <c r="U48">
+        <v>260.3549877483315</v>
+      </c>
+      <c r="V48">
+        <v>30.98958333333333</v>
+      </c>
+      <c r="W48">
+        <v>4566.8816076</v>
+      </c>
       <c r="X48" t="s">
         <v>131</v>
       </c>
+      <c r="Y48">
+        <v>260.3549877483315</v>
+      </c>
+      <c r="Z48">
+        <v>242.3549877483315</v>
+      </c>
+      <c r="AA48">
+        <v>18</v>
+      </c>
+      <c r="AB48">
+        <v>18</v>
+      </c>
+      <c r="AC48">
+        <v>438</v>
+      </c>
+      <c r="AD48">
+        <v>6.506139241770216</v>
+      </c>
+      <c r="AE48">
+        <v>0</v>
+      </c>
+      <c r="AF48">
+        <v>0</v>
+      </c>
+      <c r="AG48">
+        <v>0.1213210647200964</v>
+      </c>
+      <c r="AH48">
+        <v>0.1213210647200964</v>
+      </c>
+      <c r="AI48">
+        <v>0.112933366125005</v>
+      </c>
+      <c r="AK48">
+        <v>105.50034</v>
+      </c>
+      <c r="AL48">
+        <v>136.8546477483315</v>
+      </c>
+      <c r="AN48">
+        <v>54.59899159663865</v>
+      </c>
+      <c r="AO48">
+        <v>1615.704738151263</v>
+      </c>
+      <c r="AP48">
+        <v>530.295120562511</v>
+      </c>
+      <c r="AQ48">
+        <v>2145.999858713773</v>
+      </c>
+      <c r="AR48">
+        <v>1110.784748030245</v>
+      </c>
+      <c r="AS48">
+        <v>1144.690231635854</v>
+      </c>
+      <c r="AT48">
+        <v>83.3926483935527</v>
+      </c>
+      <c r="AU48">
+        <v>149.9715092063018</v>
+      </c>
+      <c r="AV48">
+        <v>13.11686145797029</v>
+      </c>
+      <c r="AW48">
+        <v>175.8339</v>
+      </c>
+      <c r="AX48">
+        <v>0</v>
+      </c>
+      <c r="AY48">
+        <v>0</v>
+      </c>
+      <c r="AZ48">
+        <v>-13.0012</v>
+      </c>
+      <c r="BA48">
+        <v>14.71709999999999</v>
+      </c>
+      <c r="BB48">
+        <v>0</v>
+      </c>
+      <c r="BC48">
+        <v>0</v>
+      </c>
     </row>
-    <row r="49" spans="1:24">
+    <row r="49" spans="1:55">
       <c r="A49" s="1">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C49" t="s">
         <v>57</v>
@@ -7662,16 +8115,112 @@
       <c r="R49" t="s">
         <v>83</v>
       </c>
+      <c r="U49">
+        <v>284.9565950485669</v>
+      </c>
+      <c r="V49">
+        <v>30.98958333333333</v>
+      </c>
+      <c r="W49">
+        <v>2651.235708</v>
+      </c>
       <c r="X49" t="s">
         <v>132</v>
       </c>
+      <c r="Y49">
+        <v>284.9565950485669</v>
+      </c>
+      <c r="Z49">
+        <v>266.9565950485669</v>
+      </c>
+      <c r="AA49">
+        <v>18</v>
+      </c>
+      <c r="AB49">
+        <v>18</v>
+      </c>
+      <c r="AC49">
+        <v>438</v>
+      </c>
+      <c r="AD49">
+        <v>6.506139241770216</v>
+      </c>
+      <c r="AE49">
+        <v>0</v>
+      </c>
+      <c r="AF49">
+        <v>0</v>
+      </c>
+      <c r="AG49">
+        <v>0.1327850017750508</v>
+      </c>
+      <c r="AH49">
+        <v>0.1327850017750508</v>
+      </c>
+      <c r="AI49">
+        <v>0.1243973031799593</v>
+      </c>
+      <c r="AK49">
+        <v>82.82579859399051</v>
+      </c>
+      <c r="AL49">
+        <v>184.1307964545764</v>
+      </c>
+      <c r="AN49">
+        <v>54.59899159663865</v>
+      </c>
+      <c r="AO49">
+        <v>1615.704738151263</v>
+      </c>
+      <c r="AP49">
+        <v>530.2951205625095</v>
+      </c>
+      <c r="AQ49">
+        <v>2145.999858713772</v>
+      </c>
+      <c r="AR49">
+        <v>1110.784748030245</v>
+      </c>
+      <c r="AS49">
+        <v>1050.96200448077</v>
+      </c>
+      <c r="AT49">
+        <v>10.15305457700342</v>
+      </c>
+      <c r="AU49">
+        <v>185.1378177561841</v>
+      </c>
+      <c r="AV49">
+        <v>1.007021301607659</v>
+      </c>
+      <c r="AW49">
+        <v>138.0429976566509</v>
+      </c>
+      <c r="AX49">
+        <v>0</v>
+      </c>
+      <c r="AY49">
+        <v>0</v>
+      </c>
+      <c r="AZ49">
+        <v>0</v>
+      </c>
+      <c r="BA49">
+        <v>0</v>
+      </c>
+      <c r="BB49">
+        <v>0</v>
+      </c>
+      <c r="BC49">
+        <v>0</v>
+      </c>
     </row>
-    <row r="50" spans="1:24">
+    <row r="50" spans="1:55">
       <c r="A50" s="1">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C50" t="s">
         <v>57</v>
@@ -7721,16 +8270,112 @@
       <c r="R50" t="s">
         <v>82</v>
       </c>
+      <c r="U50">
+        <v>279.8067891908049</v>
+      </c>
+      <c r="V50">
+        <v>29.98958333333333</v>
+      </c>
+      <c r="W50">
+        <v>4451.632740900004</v>
+      </c>
       <c r="X50" t="s">
         <v>133</v>
       </c>
+      <c r="Y50">
+        <v>279.8067891908049</v>
+      </c>
+      <c r="Z50">
+        <v>261.8067891908049</v>
+      </c>
+      <c r="AA50">
+        <v>18</v>
+      </c>
+      <c r="AB50">
+        <v>18</v>
+      </c>
+      <c r="AC50">
+        <v>438</v>
+      </c>
+      <c r="AD50">
+        <v>6.406199293914408</v>
+      </c>
+      <c r="AE50">
+        <v>0</v>
+      </c>
+      <c r="AF50">
+        <v>0</v>
+      </c>
+      <c r="AG50">
+        <v>0.1251552813233601</v>
+      </c>
+      <c r="AH50">
+        <v>0.1251552813233601</v>
+      </c>
+      <c r="AI50">
+        <v>0.117104028991937</v>
+      </c>
+      <c r="AK50">
+        <v>88.56148183918201</v>
+      </c>
+      <c r="AL50">
+        <v>173.2453073516228</v>
+      </c>
+      <c r="AN50">
+        <v>64.35567905522751</v>
+      </c>
+      <c r="AO50">
+        <v>1640.910548940604</v>
+      </c>
+      <c r="AP50">
+        <v>594.7664934678277</v>
+      </c>
+      <c r="AQ50">
+        <v>2235.677042408432</v>
+      </c>
+      <c r="AR50">
+        <v>987.6318419771399</v>
+      </c>
+      <c r="AS50">
+        <v>1285.964522065928</v>
+      </c>
+      <c r="AT50">
+        <v>14.39977265977131</v>
+      </c>
+      <c r="AU50">
+        <v>175.7741389441223</v>
+      </c>
+      <c r="AV50">
+        <v>2.5288315924995</v>
+      </c>
+      <c r="AW50">
+        <v>147.60246973197</v>
+      </c>
+      <c r="AX50">
+        <v>0</v>
+      </c>
+      <c r="AY50">
+        <v>0</v>
+      </c>
+      <c r="AZ50">
+        <v>0</v>
+      </c>
+      <c r="BA50">
+        <v>0</v>
+      </c>
+      <c r="BB50">
+        <v>0</v>
+      </c>
+      <c r="BC50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="51" spans="1:24">
+    <row r="51" spans="1:55">
       <c r="A51" s="1">
         <v>50</v>
       </c>
-      <c r="B51">
-        <v>0</v>
+      <c r="B51" t="s">
+        <v>55</v>
       </c>
       <c r="C51" t="s">
         <v>57</v>
@@ -7780,13 +8425,112 @@
       <c r="R51" t="s">
         <v>82</v>
       </c>
+      <c r="U51">
+        <v>292.7564720699156</v>
+      </c>
+      <c r="V51">
+        <v>29.98958333333333</v>
+      </c>
+      <c r="W51">
+        <v>4233.507264899996</v>
+      </c>
+      <c r="X51" t="s">
+        <v>134</v>
+      </c>
+      <c r="Y51">
+        <v>292.7564720699156</v>
+      </c>
+      <c r="Z51">
+        <v>274.7564720699156</v>
+      </c>
+      <c r="AA51">
+        <v>18</v>
+      </c>
+      <c r="AB51">
+        <v>18</v>
+      </c>
+      <c r="AC51">
+        <v>438</v>
+      </c>
+      <c r="AD51">
+        <v>6.406199293914408</v>
+      </c>
+      <c r="AE51">
+        <v>0</v>
+      </c>
+      <c r="AF51">
+        <v>0</v>
+      </c>
+      <c r="AG51">
+        <v>0.1309475682384506</v>
+      </c>
+      <c r="AH51">
+        <v>0.1309475682384506</v>
+      </c>
+      <c r="AI51">
+        <v>0.1228963159070275</v>
+      </c>
+      <c r="AK51">
+        <v>107.68123944</v>
+      </c>
+      <c r="AL51">
+        <v>167.0752326299155</v>
+      </c>
+      <c r="AN51">
+        <v>64.35567905522751</v>
+      </c>
+      <c r="AO51">
+        <v>1640.910548940604</v>
+      </c>
+      <c r="AP51">
+        <v>594.7664934678285</v>
+      </c>
+      <c r="AQ51">
+        <v>2235.677042408432</v>
+      </c>
+      <c r="AR51">
+        <v>987.6318419771399</v>
+      </c>
+      <c r="AS51">
+        <v>1312.3885158198</v>
+      </c>
+      <c r="AT51">
+        <v>38.4001684785129</v>
+      </c>
+      <c r="AU51">
+        <v>172.5188796019045</v>
+      </c>
+      <c r="AV51">
+        <v>5.443646971988997</v>
+      </c>
+      <c r="AW51">
+        <v>179.4687324</v>
+      </c>
+      <c r="AX51">
+        <v>0</v>
+      </c>
+      <c r="AY51">
+        <v>0</v>
+      </c>
+      <c r="AZ51">
+        <v>-15.2578629</v>
+      </c>
+      <c r="BA51">
+        <v>13.17740139999999</v>
+      </c>
+      <c r="BB51">
+        <v>0</v>
+      </c>
+      <c r="BC51">
+        <v>0</v>
+      </c>
     </row>
-    <row r="52" spans="1:24">
+    <row r="52" spans="1:55">
       <c r="A52" s="1">
         <v>51</v>
       </c>
-      <c r="B52">
-        <v>0</v>
+      <c r="B52" t="s">
+        <v>55</v>
       </c>
       <c r="C52" t="s">
         <v>57</v>
@@ -7842,13 +8586,112 @@
       <c r="T52">
         <v>0.03</v>
       </c>
+      <c r="U52">
+        <v>295.4744262699326</v>
+      </c>
+      <c r="V52">
+        <v>29.98958333333333</v>
+      </c>
+      <c r="W52">
+        <v>3864.145781399999</v>
+      </c>
+      <c r="X52" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y52">
+        <v>295.4744262699326</v>
+      </c>
+      <c r="Z52">
+        <v>277.4744262699326</v>
+      </c>
+      <c r="AA52">
+        <v>18</v>
+      </c>
+      <c r="AB52">
+        <v>18</v>
+      </c>
+      <c r="AC52">
+        <v>438</v>
+      </c>
+      <c r="AD52">
+        <v>6.406199293914408</v>
+      </c>
+      <c r="AE52">
+        <v>0</v>
+      </c>
+      <c r="AF52">
+        <v>0</v>
+      </c>
+      <c r="AG52">
+        <v>0.1321632868545389</v>
+      </c>
+      <c r="AH52">
+        <v>0.1321632868545389</v>
+      </c>
+      <c r="AI52">
+        <v>0.1241120345231158</v>
+      </c>
+      <c r="AK52">
+        <v>106.4286694238621</v>
+      </c>
+      <c r="AL52">
+        <v>171.0457568460705</v>
+      </c>
+      <c r="AN52">
+        <v>64.35567905522751</v>
+      </c>
+      <c r="AO52">
+        <v>1640.910548940604</v>
+      </c>
+      <c r="AP52">
+        <v>594.7664934678266</v>
+      </c>
+      <c r="AQ52">
+        <v>2235.677042408431</v>
+      </c>
+      <c r="AR52">
+        <v>987.6318419771399</v>
+      </c>
+      <c r="AS52">
+        <v>1297.827850434747</v>
+      </c>
+      <c r="AT52">
+        <v>23.27808072212733</v>
+      </c>
+      <c r="AU52">
+        <v>174.613785218566</v>
+      </c>
+      <c r="AV52">
+        <v>3.568028372495485</v>
+      </c>
+      <c r="AW52">
+        <v>177.3811157064368</v>
+      </c>
+      <c r="AX52">
+        <v>3.552713678800501E-15</v>
+      </c>
+      <c r="AY52">
+        <v>6.023546448786179E-16</v>
+      </c>
+      <c r="AZ52">
+        <v>-10.04302889505402</v>
+      </c>
+      <c r="BA52">
+        <v>10.82110353986559</v>
+      </c>
+      <c r="BB52">
+        <v>0</v>
+      </c>
+      <c r="BC52">
+        <v>0</v>
+      </c>
     </row>
-    <row r="53" spans="1:24">
+    <row r="53" spans="1:55">
       <c r="A53" s="1">
         <v>52</v>
       </c>
-      <c r="B53">
-        <v>0</v>
+      <c r="B53" t="s">
+        <v>55</v>
       </c>
       <c r="C53" t="s">
         <v>57</v>
@@ -7898,13 +8741,112 @@
       <c r="R53" t="s">
         <v>82</v>
       </c>
+      <c r="U53">
+        <v>291.7210463670705</v>
+      </c>
+      <c r="V53">
+        <v>29.98958333333333</v>
+      </c>
+      <c r="W53">
+        <v>3933.365212500001</v>
+      </c>
+      <c r="X53" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y53">
+        <v>291.7210463670705</v>
+      </c>
+      <c r="Z53">
+        <v>273.7210463670705</v>
+      </c>
+      <c r="AA53">
+        <v>18</v>
+      </c>
+      <c r="AB53">
+        <v>18</v>
+      </c>
+      <c r="AC53">
+        <v>438</v>
+      </c>
+      <c r="AD53">
+        <v>6.406199293914408</v>
+      </c>
+      <c r="AE53">
+        <v>0</v>
+      </c>
+      <c r="AF53">
+        <v>0</v>
+      </c>
+      <c r="AG53">
+        <v>0.1304844308160035</v>
+      </c>
+      <c r="AH53">
+        <v>0.1304844308160035</v>
+      </c>
+      <c r="AI53">
+        <v>0.1224331784845804</v>
+      </c>
+      <c r="AK53">
+        <v>106.248898163098</v>
+      </c>
+      <c r="AL53">
+        <v>167.4721482039724</v>
+      </c>
+      <c r="AN53">
+        <v>64.35567905522751</v>
+      </c>
+      <c r="AO53">
+        <v>1640.910548940604</v>
+      </c>
+      <c r="AP53">
+        <v>594.7664934678284</v>
+      </c>
+      <c r="AQ53">
+        <v>2235.677042408432</v>
+      </c>
+      <c r="AR53">
+        <v>987.6318419771399</v>
+      </c>
+      <c r="AS53">
+        <v>1303.865392640163</v>
+      </c>
+      <c r="AT53">
+        <v>29.98702222517237</v>
+      </c>
+      <c r="AU53">
+        <v>172.1772977655354</v>
+      </c>
+      <c r="AV53">
+        <v>4.705149561562921</v>
+      </c>
+      <c r="AW53">
+        <v>177.0814969384967</v>
+      </c>
+      <c r="AX53">
+        <v>0</v>
+      </c>
+      <c r="AY53">
+        <v>0</v>
+      </c>
+      <c r="AZ53">
+        <v>-11.5999000202558</v>
+      </c>
+      <c r="BA53">
+        <v>15.29257621962125</v>
+      </c>
+      <c r="BB53">
+        <v>0</v>
+      </c>
+      <c r="BC53">
+        <v>0</v>
+      </c>
     </row>
-    <row r="54" spans="1:24">
+    <row r="54" spans="1:55">
       <c r="A54" s="1">
         <v>53</v>
       </c>
-      <c r="B54">
-        <v>0</v>
+      <c r="B54" t="s">
+        <v>55</v>
       </c>
       <c r="C54" t="s">
         <v>57</v>
@@ -7954,13 +8896,112 @@
       <c r="R54" t="s">
         <v>82</v>
       </c>
+      <c r="U54">
+        <v>291.4950633520672</v>
+      </c>
+      <c r="V54">
+        <v>29.98958333333333</v>
+      </c>
+      <c r="W54">
+        <v>5353.405958700001</v>
+      </c>
+      <c r="X54" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y54">
+        <v>291.4950633520672</v>
+      </c>
+      <c r="Z54">
+        <v>273.4950633520672</v>
+      </c>
+      <c r="AA54">
+        <v>18</v>
+      </c>
+      <c r="AB54">
+        <v>18</v>
+      </c>
+      <c r="AC54">
+        <v>438</v>
+      </c>
+      <c r="AD54">
+        <v>6.406199293914408</v>
+      </c>
+      <c r="AE54">
+        <v>0</v>
+      </c>
+      <c r="AF54">
+        <v>0</v>
+      </c>
+      <c r="AG54">
+        <v>0.1303833504673142</v>
+      </c>
+      <c r="AH54">
+        <v>0.1303833504673142</v>
+      </c>
+      <c r="AI54">
+        <v>0.1223320981358911</v>
+      </c>
+      <c r="AK54">
+        <v>105.43656</v>
+      </c>
+      <c r="AL54">
+        <v>168.0585033520672</v>
+      </c>
+      <c r="AN54">
+        <v>64.35567905522751</v>
+      </c>
+      <c r="AO54">
+        <v>1640.910548940604</v>
+      </c>
+      <c r="AP54">
+        <v>594.7664934678285</v>
+      </c>
+      <c r="AQ54">
+        <v>2235.677042408432</v>
+      </c>
+      <c r="AR54">
+        <v>987.6318419771399</v>
+      </c>
+      <c r="AS54">
+        <v>1304.637381713183</v>
+      </c>
+      <c r="AT54">
+        <v>30.90425842165865</v>
+      </c>
+      <c r="AU54">
+        <v>173.0131392577902</v>
+      </c>
+      <c r="AV54">
+        <v>4.954635905723038</v>
+      </c>
+      <c r="AW54">
+        <v>175.7276</v>
+      </c>
+      <c r="AX54">
+        <v>0</v>
+      </c>
+      <c r="AY54">
+        <v>0</v>
+      </c>
+      <c r="AZ54">
+        <v>-14.2308</v>
+      </c>
+      <c r="BA54">
+        <v>17.12100000000001</v>
+      </c>
+      <c r="BB54">
+        <v>0</v>
+      </c>
+      <c r="BC54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:24">
+    <row r="55" spans="1:55">
       <c r="A55" s="1">
         <v>54</v>
       </c>
-      <c r="B55">
-        <v>0</v>
+      <c r="B55" t="s">
+        <v>55</v>
       </c>
       <c r="C55" t="s">
         <v>57</v>
@@ -8010,13 +9051,112 @@
       <c r="R55" t="s">
         <v>83</v>
       </c>
+      <c r="U55">
+        <v>348.3531467499972</v>
+      </c>
+      <c r="V55">
+        <v>29.98958333333333</v>
+      </c>
+      <c r="W55">
+        <v>2549.584180600003</v>
+      </c>
+      <c r="X55" t="s">
+        <v>138</v>
+      </c>
+      <c r="Y55">
+        <v>348.3531467499972</v>
+      </c>
+      <c r="Z55">
+        <v>330.3531467499972</v>
+      </c>
+      <c r="AA55">
+        <v>18</v>
+      </c>
+      <c r="AB55">
+        <v>18</v>
+      </c>
+      <c r="AC55">
+        <v>438</v>
+      </c>
+      <c r="AD55">
+        <v>6.406199293914408</v>
+      </c>
+      <c r="AE55">
+        <v>0</v>
+      </c>
+      <c r="AF55">
+        <v>0</v>
+      </c>
+      <c r="AG55">
+        <v>0.1558155047183051</v>
+      </c>
+      <c r="AH55">
+        <v>0.1558155047183051</v>
+      </c>
+      <c r="AI55">
+        <v>0.147764252386882</v>
+      </c>
+      <c r="AK55">
+        <v>108.7429839565256</v>
+      </c>
+      <c r="AL55">
+        <v>221.6101627934716</v>
+      </c>
+      <c r="AN55">
+        <v>64.35567905522751</v>
+      </c>
+      <c r="AO55">
+        <v>1640.910548940604</v>
+      </c>
+      <c r="AP55">
+        <v>594.7664934678266</v>
+      </c>
+      <c r="AQ55">
+        <v>2235.677042408431</v>
+      </c>
+      <c r="AR55">
+        <v>987.6318419771399</v>
+      </c>
+      <c r="AS55">
+        <v>1252.275043262551</v>
+      </c>
+      <c r="AT55">
+        <v>6.041711070304707E-15</v>
+      </c>
+      <c r="AU55">
+        <v>221.6101627934716</v>
+      </c>
+      <c r="AV55">
+        <v>4.94580687623598E-16</v>
+      </c>
+      <c r="AW55">
+        <v>181.2383065942093</v>
+      </c>
+      <c r="AX55">
+        <v>0</v>
+      </c>
+      <c r="AY55">
+        <v>0</v>
+      </c>
+      <c r="AZ55">
+        <v>0</v>
+      </c>
+      <c r="BA55">
+        <v>0</v>
+      </c>
+      <c r="BB55">
+        <v>0</v>
+      </c>
+      <c r="BC55">
+        <v>0</v>
+      </c>
     </row>
-    <row r="56" spans="1:24">
+    <row r="56" spans="1:55">
       <c r="A56" s="1">
         <v>55</v>
       </c>
-      <c r="B56">
-        <v>0</v>
+      <c r="B56" t="s">
+        <v>55</v>
       </c>
       <c r="C56" t="s">
         <v>57</v>
@@ -8066,13 +9206,112 @@
       <c r="R56" t="s">
         <v>82</v>
       </c>
+      <c r="U56">
+        <v>339.9099808382465</v>
+      </c>
+      <c r="V56">
+        <v>30.98958333333333</v>
+      </c>
+      <c r="W56">
+        <v>5697.386394699999</v>
+      </c>
+      <c r="X56" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y56">
+        <v>339.9099808382465</v>
+      </c>
+      <c r="Z56">
+        <v>321.9099808382465</v>
+      </c>
+      <c r="AA56">
+        <v>18</v>
+      </c>
+      <c r="AB56">
+        <v>18</v>
+      </c>
+      <c r="AC56">
+        <v>438</v>
+      </c>
+      <c r="AD56">
+        <v>5.64777870663823</v>
+      </c>
+      <c r="AE56">
+        <v>0</v>
+      </c>
+      <c r="AF56">
+        <v>0</v>
+      </c>
+      <c r="AG56">
+        <v>0.1262058737853989</v>
+      </c>
+      <c r="AH56">
+        <v>0.1262058737853989</v>
+      </c>
+      <c r="AI56">
+        <v>0.1195226168756283</v>
+      </c>
+      <c r="AK56">
+        <v>80.86705990883932</v>
+      </c>
+      <c r="AL56">
+        <v>251.3858279808227</v>
+      </c>
+      <c r="AN56">
+        <v>91.74050420168068</v>
+      </c>
+      <c r="AO56">
+        <v>1861.262727529411</v>
+      </c>
+      <c r="AP56">
+        <v>832.0349031040985</v>
+      </c>
+      <c r="AQ56">
+        <v>2693.297630633509</v>
+      </c>
+      <c r="AR56">
+        <v>932.8271981736434</v>
+      </c>
+      <c r="AS56">
+        <v>1787.098664323864</v>
+      </c>
+      <c r="AT56">
+        <v>1.10288652160475E-14</v>
+      </c>
+      <c r="AU56">
+        <v>251.3858279808227</v>
+      </c>
+      <c r="AV56">
+        <v>1.430315104003324E-15</v>
+      </c>
+      <c r="AW56">
+        <v>134.7784331813989</v>
+      </c>
+      <c r="AX56">
+        <v>61.00298268443759</v>
+      </c>
+      <c r="AY56">
+        <v>10.34290705141554</v>
+      </c>
+      <c r="AZ56">
+        <v>0</v>
+      </c>
+      <c r="BA56">
+        <v>0</v>
+      </c>
+      <c r="BB56">
+        <v>0</v>
+      </c>
+      <c r="BC56">
+        <v>0</v>
+      </c>
     </row>
-    <row r="57" spans="1:24">
+    <row r="57" spans="1:55">
       <c r="A57" s="1">
         <v>56</v>
       </c>
-      <c r="B57">
-        <v>0</v>
+      <c r="B57" t="s">
+        <v>55</v>
       </c>
       <c r="C57" t="s">
         <v>57</v>
@@ -8122,13 +9361,112 @@
       <c r="R57" t="s">
         <v>82</v>
       </c>
+      <c r="U57">
+        <v>379.5842343396458</v>
+      </c>
+      <c r="V57">
+        <v>30.98958333333333</v>
+      </c>
+      <c r="W57">
+        <v>6370.666004500003</v>
+      </c>
+      <c r="X57" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y57">
+        <v>379.5842343396458</v>
+      </c>
+      <c r="Z57">
+        <v>361.5842343396458</v>
+      </c>
+      <c r="AA57">
+        <v>18</v>
+      </c>
+      <c r="AB57">
+        <v>18</v>
+      </c>
+      <c r="AC57">
+        <v>438</v>
+      </c>
+      <c r="AD57">
+        <v>5.64777870663823</v>
+      </c>
+      <c r="AE57">
+        <v>0</v>
+      </c>
+      <c r="AF57">
+        <v>0</v>
+      </c>
+      <c r="AG57">
+        <v>0.1409366087216886</v>
+      </c>
+      <c r="AH57">
+        <v>0.1409366087216886</v>
+      </c>
+      <c r="AI57">
+        <v>0.1342533518119181</v>
+      </c>
+      <c r="AK57">
+        <v>116.4712629</v>
+      </c>
+      <c r="AL57">
+        <v>245.1129714396458</v>
+      </c>
+      <c r="AN57">
+        <v>91.74050420168068</v>
+      </c>
+      <c r="AO57">
+        <v>1861.262727529411</v>
+      </c>
+      <c r="AP57">
+        <v>832.0349031040981</v>
+      </c>
+      <c r="AQ57">
+        <v>2693.297630633509</v>
+      </c>
+      <c r="AR57">
+        <v>932.8271981736434</v>
+      </c>
+      <c r="AS57">
+        <v>1796.756024848255</v>
+      </c>
+      <c r="AT57">
+        <v>10.07151732154984</v>
+      </c>
+      <c r="AU57">
+        <v>246.3404980861127</v>
+      </c>
+      <c r="AV57">
+        <v>1.227526646466891</v>
+      </c>
+      <c r="AW57">
+        <v>194.1187715</v>
+      </c>
+      <c r="AX57">
+        <v>0</v>
+      </c>
+      <c r="AY57">
+        <v>0</v>
+      </c>
+      <c r="AZ57">
+        <v>-8.451232900000001</v>
+      </c>
+      <c r="BA57">
+        <v>25.23137149999999</v>
+      </c>
+      <c r="BB57">
+        <v>0</v>
+      </c>
+      <c r="BC57">
+        <v>0</v>
+      </c>
     </row>
-    <row r="58" spans="1:24">
+    <row r="58" spans="1:55">
       <c r="A58" s="1">
         <v>57</v>
       </c>
-      <c r="B58">
-        <v>0</v>
+      <c r="B58" t="s">
+        <v>55</v>
       </c>
       <c r="C58" t="s">
         <v>57</v>
@@ -8184,13 +9522,112 @@
       <c r="T58">
         <v>0.03</v>
       </c>
+      <c r="U58">
+        <v>376.8551578332443</v>
+      </c>
+      <c r="V58">
+        <v>30.98958333333333</v>
+      </c>
+      <c r="W58">
+        <v>6908.566223300004</v>
+      </c>
+      <c r="X58" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y58">
+        <v>376.8551578332443</v>
+      </c>
+      <c r="Z58">
+        <v>358.8551578332443</v>
+      </c>
+      <c r="AA58">
+        <v>18</v>
+      </c>
+      <c r="AB58">
+        <v>18</v>
+      </c>
+      <c r="AC58">
+        <v>438</v>
+      </c>
+      <c r="AD58">
+        <v>5.64777870663823</v>
+      </c>
+      <c r="AE58">
+        <v>0</v>
+      </c>
+      <c r="AF58">
+        <v>0</v>
+      </c>
+      <c r="AG58">
+        <v>0.1399233243095385</v>
+      </c>
+      <c r="AH58">
+        <v>0.1399233243095385</v>
+      </c>
+      <c r="AI58">
+        <v>0.133240067399768</v>
+      </c>
+      <c r="AK58">
+        <v>107.058181939027</v>
+      </c>
+      <c r="AL58">
+        <v>251.7969758942173</v>
+      </c>
+      <c r="AN58">
+        <v>91.74050420168068</v>
+      </c>
+      <c r="AO58">
+        <v>1861.262727529411</v>
+      </c>
+      <c r="AP58">
+        <v>832.0349031040996</v>
+      </c>
+      <c r="AQ58">
+        <v>2693.29763063351</v>
+      </c>
+      <c r="AR58">
+        <v>932.8271981736434</v>
+      </c>
+      <c r="AS58">
+        <v>1795.472260451524</v>
+      </c>
+      <c r="AT58">
+        <v>8.031557413393195</v>
+      </c>
+      <c r="AU58">
+        <v>252.8780922538922</v>
+      </c>
+      <c r="AV58">
+        <v>1.081116359674888</v>
+      </c>
+      <c r="AW58">
+        <v>178.4303032317117</v>
+      </c>
+      <c r="AX58">
+        <v>0</v>
+      </c>
+      <c r="AY58">
+        <v>0</v>
+      </c>
+      <c r="AZ58">
+        <v>-13.32749125504222</v>
+      </c>
+      <c r="BA58">
+        <v>12.04276345426355</v>
+      </c>
+      <c r="BB58">
+        <v>0</v>
+      </c>
+      <c r="BC58">
+        <v>0</v>
+      </c>
     </row>
-    <row r="59" spans="1:24">
+    <row r="59" spans="1:55">
       <c r="A59" s="1">
         <v>58</v>
       </c>
-      <c r="B59">
-        <v>0</v>
+      <c r="B59" t="s">
+        <v>55</v>
       </c>
       <c r="C59" t="s">
         <v>57</v>
@@ -8240,13 +9677,112 @@
       <c r="R59" t="s">
         <v>82</v>
       </c>
+      <c r="U59">
+        <v>371.0863959368644</v>
+      </c>
+      <c r="V59">
+        <v>30.98958333333333</v>
+      </c>
+      <c r="W59">
+        <v>4959.816558400002</v>
+      </c>
+      <c r="X59" t="s">
+        <v>142</v>
+      </c>
+      <c r="Y59">
+        <v>371.0863959368644</v>
+      </c>
+      <c r="Z59">
+        <v>353.0863959368644</v>
+      </c>
+      <c r="AA59">
+        <v>18</v>
+      </c>
+      <c r="AB59">
+        <v>18</v>
+      </c>
+      <c r="AC59">
+        <v>438</v>
+      </c>
+      <c r="AD59">
+        <v>5.64777870663823</v>
+      </c>
+      <c r="AE59">
+        <v>0</v>
+      </c>
+      <c r="AF59">
+        <v>0</v>
+      </c>
+      <c r="AG59">
+        <v>0.1377814288759384</v>
+      </c>
+      <c r="AH59">
+        <v>0.1377814288759384</v>
+      </c>
+      <c r="AI59">
+        <v>0.1310981719661679</v>
+      </c>
+      <c r="AK59">
+        <v>108.1378678442093</v>
+      </c>
+      <c r="AL59">
+        <v>244.9485280926551</v>
+      </c>
+      <c r="AN59">
+        <v>91.74050420168068</v>
+      </c>
+      <c r="AO59">
+        <v>1861.262727529411</v>
+      </c>
+      <c r="AP59">
+        <v>832.0349031040992</v>
+      </c>
+      <c r="AQ59">
+        <v>2693.29763063351</v>
+      </c>
+      <c r="AR59">
+        <v>932.8271981736434</v>
+      </c>
+      <c r="AS59">
+        <v>1789.767882400403</v>
+      </c>
+      <c r="AT59">
+        <v>3.095472118295333</v>
+      </c>
+      <c r="AU59">
+        <v>245.3996782861724</v>
+      </c>
+      <c r="AV59">
+        <v>0.4511501935172536</v>
+      </c>
+      <c r="AW59">
+        <v>180.2297797403488</v>
+      </c>
+      <c r="AX59">
+        <v>0</v>
+      </c>
+      <c r="AY59">
+        <v>0</v>
+      </c>
+      <c r="AZ59">
+        <v>-12.71181636181905</v>
+      </c>
+      <c r="BA59">
+        <v>11.8668929871788</v>
+      </c>
+      <c r="BB59">
+        <v>0</v>
+      </c>
+      <c r="BC59">
+        <v>0</v>
+      </c>
     </row>
-    <row r="60" spans="1:24">
+    <row r="60" spans="1:55">
       <c r="A60" s="1">
         <v>59</v>
       </c>
-      <c r="B60">
-        <v>0</v>
+      <c r="B60" t="s">
+        <v>55</v>
       </c>
       <c r="C60" t="s">
         <v>57</v>
@@ -8296,13 +9832,112 @@
       <c r="R60" t="s">
         <v>82</v>
       </c>
+      <c r="U60">
+        <v>372.3516910614026</v>
+      </c>
+      <c r="V60">
+        <v>30.98958333333333</v>
+      </c>
+      <c r="W60">
+        <v>6275.370846099999</v>
+      </c>
+      <c r="X60" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y60">
+        <v>372.3516910614026</v>
+      </c>
+      <c r="Z60">
+        <v>354.3516910614026</v>
+      </c>
+      <c r="AA60">
+        <v>18</v>
+      </c>
+      <c r="AB60">
+        <v>18</v>
+      </c>
+      <c r="AC60">
+        <v>438</v>
+      </c>
+      <c r="AD60">
+        <v>5.64777870663823</v>
+      </c>
+      <c r="AE60">
+        <v>0</v>
+      </c>
+      <c r="AF60">
+        <v>0</v>
+      </c>
+      <c r="AG60">
+        <v>0.1382512228972701</v>
+      </c>
+      <c r="AH60">
+        <v>0.1382512228972701</v>
+      </c>
+      <c r="AI60">
+        <v>0.1315679659874995</v>
+      </c>
+      <c r="AK60">
+        <v>108.11478</v>
+      </c>
+      <c r="AL60">
+        <v>246.2369110614025</v>
+      </c>
+      <c r="AN60">
+        <v>91.74050420168068</v>
+      </c>
+      <c r="AO60">
+        <v>1861.262727529411</v>
+      </c>
+      <c r="AP60">
+        <v>832.0349031040978</v>
+      </c>
+      <c r="AQ60">
+        <v>2693.297630633509</v>
+      </c>
+      <c r="AR60">
+        <v>932.8271981736434</v>
+      </c>
+      <c r="AS60">
+        <v>1793.102932933401</v>
+      </c>
+      <c r="AT60">
+        <v>6.494665220806609</v>
+      </c>
+      <c r="AU60">
+        <v>247.1650207975077</v>
+      </c>
+      <c r="AV60">
+        <v>0.928109736105134</v>
+      </c>
+      <c r="AW60">
+        <v>180.1913</v>
+      </c>
+      <c r="AX60">
+        <v>7.105427357601002E-15</v>
+      </c>
+      <c r="AY60">
+        <v>1.204707892733915E-15</v>
+      </c>
+      <c r="AZ60">
+        <v>-16.59869999999999</v>
+      </c>
+      <c r="BA60">
+        <v>15.94899999999999</v>
+      </c>
+      <c r="BB60">
+        <v>0</v>
+      </c>
+      <c r="BC60">
+        <v>0</v>
+      </c>
     </row>
-    <row r="61" spans="1:24">
+    <row r="61" spans="1:55">
       <c r="A61" s="1">
         <v>60</v>
       </c>
-      <c r="B61">
-        <v>0</v>
+      <c r="B61" t="s">
+        <v>55</v>
       </c>
       <c r="C61" t="s">
         <v>57</v>
@@ -8352,13 +9987,112 @@
       <c r="R61" t="s">
         <v>83</v>
       </c>
+      <c r="U61">
+        <v>440.3534665142407</v>
+      </c>
+      <c r="V61">
+        <v>30.98958333333333</v>
+      </c>
+      <c r="W61">
+        <v>3227.808416500004</v>
+      </c>
+      <c r="X61" t="s">
+        <v>144</v>
+      </c>
+      <c r="Y61">
+        <v>440.3534665142407</v>
+      </c>
+      <c r="Z61">
+        <v>422.3534665142407</v>
+      </c>
+      <c r="AA61">
+        <v>18</v>
+      </c>
+      <c r="AB61">
+        <v>18</v>
+      </c>
+      <c r="AC61">
+        <v>438</v>
+      </c>
+      <c r="AD61">
+        <v>5.64777870663823</v>
+      </c>
+      <c r="AE61">
+        <v>0</v>
+      </c>
+      <c r="AF61">
+        <v>0</v>
+      </c>
+      <c r="AG61">
+        <v>0.1634997415457058</v>
+      </c>
+      <c r="AH61">
+        <v>0.1634997415457058</v>
+      </c>
+      <c r="AI61">
+        <v>0.1568164846359352</v>
+      </c>
+      <c r="AK61">
+        <v>103.1540411937717</v>
+      </c>
+      <c r="AL61">
+        <v>319.199425320469</v>
+      </c>
+      <c r="AN61">
+        <v>91.74050420168068</v>
+      </c>
+      <c r="AO61">
+        <v>1861.262727529411</v>
+      </c>
+      <c r="AP61">
+        <v>832.0349031040996</v>
+      </c>
+      <c r="AQ61">
+        <v>2693.29763063351</v>
+      </c>
+      <c r="AR61">
+        <v>932.8271981736434</v>
+      </c>
+      <c r="AS61">
+        <v>1762.218360629182</v>
+      </c>
+      <c r="AT61">
+        <v>3.854843615182527E-15</v>
+      </c>
+      <c r="AU61">
+        <v>319.199425320469</v>
+      </c>
+      <c r="AV61">
+        <v>3.394555225146606E-16</v>
+      </c>
+      <c r="AW61">
+        <v>171.9234019896195</v>
+      </c>
+      <c r="AX61">
+        <v>0</v>
+      </c>
+      <c r="AY61">
+        <v>0</v>
+      </c>
+      <c r="AZ61">
+        <v>0</v>
+      </c>
+      <c r="BA61">
+        <v>0</v>
+      </c>
+      <c r="BB61">
+        <v>0</v>
+      </c>
+      <c r="BC61">
+        <v>0</v>
+      </c>
     </row>
-    <row r="62" spans="1:24">
+    <row r="62" spans="1:55">
       <c r="A62" s="1">
         <v>61</v>
       </c>
-      <c r="B62">
-        <v>0</v>
+      <c r="B62" t="s">
+        <v>55</v>
       </c>
       <c r="C62" t="s">
         <v>57</v>
@@ -8408,13 +10142,112 @@
       <c r="R62" t="s">
         <v>82</v>
       </c>
+      <c r="U62">
+        <v>387.0368013301942</v>
+      </c>
+      <c r="V62">
+        <v>29.98958333333333</v>
+      </c>
+      <c r="W62">
+        <v>5517.785017000002</v>
+      </c>
+      <c r="X62" t="s">
+        <v>145</v>
+      </c>
+      <c r="Y62">
+        <v>387.0368013301942</v>
+      </c>
+      <c r="Z62">
+        <v>369.0368013301942</v>
+      </c>
+      <c r="AA62">
+        <v>18</v>
+      </c>
+      <c r="AB62">
+        <v>18</v>
+      </c>
+      <c r="AC62">
+        <v>438</v>
+      </c>
+      <c r="AD62">
+        <v>5.968670304251937</v>
+      </c>
+      <c r="AE62">
+        <v>0</v>
+      </c>
+      <c r="AF62">
+        <v>0</v>
+      </c>
+      <c r="AG62">
+        <v>0.1538528705178946</v>
+      </c>
+      <c r="AH62">
+        <v>0.1538528705178946</v>
+      </c>
+      <c r="AI62">
+        <v>0.1466976034740265</v>
+      </c>
+      <c r="AK62">
+        <v>101.067015513013</v>
+      </c>
+      <c r="AL62">
+        <v>267.9697858171812</v>
+      </c>
+      <c r="AN62">
+        <v>79.36088919763807</v>
+      </c>
+      <c r="AO62">
+        <v>1761.196290656481</v>
+      </c>
+      <c r="AP62">
+        <v>754.4330897207797</v>
+      </c>
+      <c r="AQ62">
+        <v>2515.629380377261</v>
+      </c>
+      <c r="AR62">
+        <v>626.1831707214252</v>
+      </c>
+      <c r="AS62">
+        <v>1914.615875829375</v>
+      </c>
+      <c r="AT62">
+        <v>0.9686625835503768</v>
+      </c>
+      <c r="AU62">
+        <v>268.1406578969195</v>
+      </c>
+      <c r="AV62">
+        <v>0.170872079738286</v>
+      </c>
+      <c r="AW62">
+        <v>168.4450258550217</v>
+      </c>
+      <c r="AX62">
+        <v>0</v>
+      </c>
+      <c r="AY62">
+        <v>0</v>
+      </c>
+      <c r="AZ62">
+        <v>0</v>
+      </c>
+      <c r="BA62">
+        <v>0</v>
+      </c>
+      <c r="BB62">
+        <v>0</v>
+      </c>
+      <c r="BC62">
+        <v>0</v>
+      </c>
     </row>
-    <row r="63" spans="1:24">
+    <row r="63" spans="1:55">
       <c r="A63" s="1">
         <v>62</v>
       </c>
-      <c r="B63">
-        <v>0</v>
+      <c r="B63" t="s">
+        <v>55</v>
       </c>
       <c r="C63" t="s">
         <v>57</v>
@@ -8464,13 +10297,112 @@
       <c r="R63" t="s">
         <v>82</v>
       </c>
+      <c r="U63">
+        <v>396.1762108619537</v>
+      </c>
+      <c r="V63">
+        <v>29.98958333333333</v>
+      </c>
+      <c r="W63">
+        <v>4971.310907800005</v>
+      </c>
+      <c r="X63" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y63">
+        <v>396.1762108619537</v>
+      </c>
+      <c r="Z63">
+        <v>378.1762108619537</v>
+      </c>
+      <c r="AA63">
+        <v>18</v>
+      </c>
+      <c r="AB63">
+        <v>18</v>
+      </c>
+      <c r="AC63">
+        <v>438</v>
+      </c>
+      <c r="AD63">
+        <v>5.968670304251937</v>
+      </c>
+      <c r="AE63">
+        <v>0</v>
+      </c>
+      <c r="AF63">
+        <v>0</v>
+      </c>
+      <c r="AG63">
+        <v>0.1574859213969509</v>
+      </c>
+      <c r="AH63">
+        <v>0.1574859213969509</v>
+      </c>
+      <c r="AI63">
+        <v>0.1503306543530827</v>
+      </c>
+      <c r="AK63">
+        <v>110.84218206</v>
+      </c>
+      <c r="AL63">
+        <v>267.3340288019537</v>
+      </c>
+      <c r="AN63">
+        <v>79.36088919763807</v>
+      </c>
+      <c r="AO63">
+        <v>1761.196290656481</v>
+      </c>
+      <c r="AP63">
+        <v>754.4330897207798</v>
+      </c>
+      <c r="AQ63">
+        <v>2515.629380377261</v>
+      </c>
+      <c r="AR63">
+        <v>626.1831707214252</v>
+      </c>
+      <c r="AS63">
+        <v>1933.022584373438</v>
+      </c>
+      <c r="AT63">
+        <v>18.56556949242909</v>
+      </c>
+      <c r="AU63">
+        <v>269.6791775044766</v>
+      </c>
+      <c r="AV63">
+        <v>2.345148702522902</v>
+      </c>
+      <c r="AW63">
+        <v>184.7369701</v>
+      </c>
+      <c r="AX63">
+        <v>0</v>
+      </c>
+      <c r="AY63">
+        <v>0</v>
+      </c>
+      <c r="AZ63">
+        <v>-62.6875752</v>
+      </c>
+      <c r="BA63">
+        <v>15.84957010000001</v>
+      </c>
+      <c r="BB63">
+        <v>0</v>
+      </c>
+      <c r="BC63">
+        <v>0</v>
+      </c>
     </row>
-    <row r="64" spans="1:24">
+    <row r="64" spans="1:55">
       <c r="A64" s="1">
         <v>63</v>
       </c>
-      <c r="B64">
-        <v>0</v>
+      <c r="B64" t="s">
+        <v>56</v>
       </c>
       <c r="C64" t="s">
         <v>57</v>
@@ -8526,13 +10458,16 @@
       <c r="T64">
         <v>0.03</v>
       </c>
+      <c r="X64" t="s">
+        <v>147</v>
+      </c>
     </row>
-    <row r="65" spans="1:20">
+    <row r="65" spans="1:55">
       <c r="A65" s="1">
         <v>64</v>
       </c>
-      <c r="B65">
-        <v>0</v>
+      <c r="B65" t="s">
+        <v>55</v>
       </c>
       <c r="C65" t="s">
         <v>57</v>
@@ -8582,13 +10517,112 @@
       <c r="R65" t="s">
         <v>82</v>
       </c>
+      <c r="U65">
+        <v>407.1938633905412</v>
+      </c>
+      <c r="V65">
+        <v>29.98958333333333</v>
+      </c>
+      <c r="W65">
+        <v>5085.127250199999</v>
+      </c>
+      <c r="X65" t="s">
+        <v>148</v>
+      </c>
+      <c r="Y65">
+        <v>407.1938633905412</v>
+      </c>
+      <c r="Z65">
+        <v>389.1938633905412</v>
+      </c>
+      <c r="AA65">
+        <v>18</v>
+      </c>
+      <c r="AB65">
+        <v>18</v>
+      </c>
+      <c r="AC65">
+        <v>438</v>
+      </c>
+      <c r="AD65">
+        <v>5.968670304251937</v>
+      </c>
+      <c r="AE65">
+        <v>0</v>
+      </c>
+      <c r="AF65">
+        <v>0</v>
+      </c>
+      <c r="AG65">
+        <v>0.1618656017324283</v>
+      </c>
+      <c r="AH65">
+        <v>0.1618656017324283</v>
+      </c>
+      <c r="AI65">
+        <v>0.1547103346885601</v>
+      </c>
+      <c r="AK65">
+        <v>122.26998</v>
+      </c>
+      <c r="AL65">
+        <v>266.9238833905412</v>
+      </c>
+      <c r="AN65">
+        <v>79.36088919763807</v>
+      </c>
+      <c r="AO65">
+        <v>1761.196290656481</v>
+      </c>
+      <c r="AP65">
+        <v>754.4330897207802</v>
+      </c>
+      <c r="AQ65">
+        <v>2515.629380377261</v>
+      </c>
+      <c r="AR65">
+        <v>626.1831707214252</v>
+      </c>
+      <c r="AS65">
+        <v>1926.371985519422</v>
+      </c>
+      <c r="AT65">
+        <v>11.82981129834623</v>
+      </c>
+      <c r="AU65">
+        <v>268.5588042196389</v>
+      </c>
+      <c r="AV65">
+        <v>1.634920829097744</v>
+      </c>
+      <c r="AW65">
+        <v>203.7833</v>
+      </c>
+      <c r="AX65">
+        <v>3.552713678800501E-15</v>
+      </c>
+      <c r="AY65">
+        <v>6.023546448786179E-16</v>
+      </c>
+      <c r="AZ65">
+        <v>-61.13808536617337</v>
+      </c>
+      <c r="BA65">
+        <v>52.16011448297026</v>
+      </c>
+      <c r="BB65">
+        <v>0</v>
+      </c>
+      <c r="BC65">
+        <v>0</v>
+      </c>
     </row>
-    <row r="66" spans="1:20">
+    <row r="66" spans="1:55">
       <c r="A66" s="1">
         <v>65</v>
       </c>
-      <c r="B66">
-        <v>0</v>
+      <c r="B66" t="s">
+        <v>55</v>
       </c>
       <c r="C66" t="s">
         <v>57</v>
@@ -8638,13 +10672,112 @@
       <c r="R66" t="s">
         <v>82</v>
       </c>
+      <c r="U66">
+        <v>402.0134982322932</v>
+      </c>
+      <c r="V66">
+        <v>29.98958333333333</v>
+      </c>
+      <c r="W66">
+        <v>4273.470481099997</v>
+      </c>
+      <c r="X66" t="s">
+        <v>149</v>
+      </c>
+      <c r="Y66">
+        <v>402.0134982322932</v>
+      </c>
+      <c r="Z66">
+        <v>384.0134982322932</v>
+      </c>
+      <c r="AA66">
+        <v>18</v>
+      </c>
+      <c r="AB66">
+        <v>18</v>
+      </c>
+      <c r="AC66">
+        <v>438</v>
+      </c>
+      <c r="AD66">
+        <v>5.968670304251937</v>
+      </c>
+      <c r="AE66">
+        <v>0</v>
+      </c>
+      <c r="AF66">
+        <v>0</v>
+      </c>
+      <c r="AG66">
+        <v>0.1598063297273164</v>
+      </c>
+      <c r="AH66">
+        <v>0.1598063297273164</v>
+      </c>
+      <c r="AI66">
+        <v>0.1526510626834482</v>
+      </c>
+      <c r="AK66">
+        <v>113.03934</v>
+      </c>
+      <c r="AL66">
+        <v>270.9741582322932</v>
+      </c>
+      <c r="AN66">
+        <v>79.36088919763807</v>
+      </c>
+      <c r="AO66">
+        <v>1761.196290656481</v>
+      </c>
+      <c r="AP66">
+        <v>754.43308972078</v>
+      </c>
+      <c r="AQ66">
+        <v>2515.629380377261</v>
+      </c>
+      <c r="AR66">
+        <v>626.1831707214252</v>
+      </c>
+      <c r="AS66">
+        <v>1922.033884251562</v>
+      </c>
+      <c r="AT66">
+        <v>8.107836303821342</v>
+      </c>
+      <c r="AU66">
+        <v>272.2212149102388</v>
+      </c>
+      <c r="AV66">
+        <v>1.247056677945495</v>
+      </c>
+      <c r="AW66">
+        <v>188.3989</v>
+      </c>
+      <c r="AX66">
+        <v>0</v>
+      </c>
+      <c r="AY66">
+        <v>0</v>
+      </c>
+      <c r="AZ66">
+        <v>-61.0537</v>
+      </c>
+      <c r="BA66">
+        <v>57.7833</v>
+      </c>
+      <c r="BB66">
+        <v>0</v>
+      </c>
+      <c r="BC66">
+        <v>0</v>
+      </c>
     </row>
-    <row r="67" spans="1:20">
+    <row r="67" spans="1:55">
       <c r="A67" s="1">
         <v>66</v>
       </c>
-      <c r="B67">
-        <v>0</v>
+      <c r="B67" t="s">
+        <v>55</v>
       </c>
       <c r="C67" t="s">
         <v>57</v>
@@ -8694,13 +10827,112 @@
       <c r="R67" t="s">
         <v>83</v>
       </c>
+      <c r="U67">
+        <v>480.1991331359791</v>
+      </c>
+      <c r="V67">
+        <v>29.98958333333333</v>
+      </c>
+      <c r="W67">
+        <v>3013.441127099999</v>
+      </c>
+      <c r="X67" t="s">
+        <v>150</v>
+      </c>
+      <c r="Y67">
+        <v>480.1991331359791</v>
+      </c>
+      <c r="Z67">
+        <v>462.1991331359791</v>
+      </c>
+      <c r="AA67">
+        <v>18</v>
+      </c>
+      <c r="AB67">
+        <v>18</v>
+      </c>
+      <c r="AC67">
+        <v>438</v>
+      </c>
+      <c r="AD67">
+        <v>5.968670304251937</v>
+      </c>
+      <c r="AE67">
+        <v>0</v>
+      </c>
+      <c r="AF67">
+        <v>0</v>
+      </c>
+      <c r="AG67">
+        <v>0.1908862795456639</v>
+      </c>
+      <c r="AH67">
+        <v>0.1908862795456639</v>
+      </c>
+      <c r="AI67">
+        <v>0.1837310125017957</v>
+      </c>
+      <c r="AK67">
+        <v>122.7362998923553</v>
+      </c>
+      <c r="AL67">
+        <v>339.4628332436238</v>
+      </c>
+      <c r="AN67">
+        <v>79.36088919763807</v>
+      </c>
+      <c r="AO67">
+        <v>1761.196290656481</v>
+      </c>
+      <c r="AP67">
+        <v>754.4330897207794</v>
+      </c>
+      <c r="AQ67">
+        <v>2515.629380377261</v>
+      </c>
+      <c r="AR67">
+        <v>626.1831707214252</v>
+      </c>
+      <c r="AS67">
+        <v>1890.98697588306</v>
+      </c>
+      <c r="AT67">
+        <v>4.312863601044721E-15</v>
+      </c>
+      <c r="AU67">
+        <v>339.4628332436238</v>
+      </c>
+      <c r="AV67">
+        <v>3.180516635054375E-16</v>
+      </c>
+      <c r="AW67">
+        <v>204.5604998205922</v>
+      </c>
+      <c r="AX67">
+        <v>0</v>
+      </c>
+      <c r="AY67">
+        <v>0</v>
+      </c>
+      <c r="AZ67">
+        <v>0</v>
+      </c>
+      <c r="BA67">
+        <v>0</v>
+      </c>
+      <c r="BB67">
+        <v>0</v>
+      </c>
+      <c r="BC67">
+        <v>0</v>
+      </c>
     </row>
-    <row r="68" spans="1:20">
+    <row r="68" spans="1:55">
       <c r="A68" s="1">
         <v>67</v>
       </c>
-      <c r="B68">
-        <v>0</v>
+      <c r="B68" t="s">
+        <v>56</v>
       </c>
       <c r="C68" t="s">
         <v>57</v>
@@ -8750,13 +10982,16 @@
       <c r="R68" t="s">
         <v>82</v>
       </c>
+      <c r="X68" t="s">
+        <v>151</v>
+      </c>
     </row>
-    <row r="69" spans="1:20">
+    <row r="69" spans="1:55">
       <c r="A69" s="1">
         <v>68</v>
       </c>
-      <c r="B69">
-        <v>0</v>
+      <c r="B69" t="s">
+        <v>55</v>
       </c>
       <c r="C69" t="s">
         <v>57</v>
@@ -8806,13 +11041,112 @@
       <c r="R69" t="s">
         <v>82</v>
       </c>
+      <c r="U69">
+        <v>353.081370355831</v>
+      </c>
+      <c r="V69">
+        <v>29.98958333333333</v>
+      </c>
+      <c r="W69">
+        <v>3531.498032299998</v>
+      </c>
+      <c r="X69" t="s">
+        <v>152</v>
+      </c>
+      <c r="Y69">
+        <v>353.081370355831</v>
+      </c>
+      <c r="Z69">
+        <v>335.081370355831</v>
+      </c>
+      <c r="AA69">
+        <v>18</v>
+      </c>
+      <c r="AB69">
+        <v>18</v>
+      </c>
+      <c r="AC69">
+        <v>438</v>
+      </c>
+      <c r="AD69">
+        <v>6.943021896517559</v>
+      </c>
+      <c r="AE69">
+        <v>0</v>
+      </c>
+      <c r="AF69">
+        <v>0</v>
+      </c>
+      <c r="AG69">
+        <v>0.1710889204359024</v>
+      </c>
+      <c r="AH69">
+        <v>0.1710889204359024</v>
+      </c>
+      <c r="AI69">
+        <v>0.1623668500396573</v>
+      </c>
+      <c r="AK69">
+        <v>115.55719158</v>
+      </c>
+      <c r="AL69">
+        <v>219.524178775831</v>
+      </c>
+      <c r="AN69">
+        <v>58.68704411253908</v>
+      </c>
+      <c r="AO69">
+        <v>1514.038146022922</v>
+      </c>
+      <c r="AP69">
+        <v>549.6920444315268</v>
+      </c>
+      <c r="AQ69">
+        <v>2063.730190454449</v>
+      </c>
+      <c r="AR69">
+        <v>475.3545887162526</v>
+      </c>
+      <c r="AS69">
+        <v>1643.108366892747</v>
+      </c>
+      <c r="AT69">
+        <v>29.3215120493901</v>
+      </c>
+      <c r="AU69">
+        <v>223.7685704340535</v>
+      </c>
+      <c r="AV69">
+        <v>4.244391658222419</v>
+      </c>
+      <c r="AW69">
+        <v>192.5953193</v>
+      </c>
+      <c r="AX69">
+        <v>2.664535259100376E-14</v>
+      </c>
+      <c r="AY69">
+        <v>4.517659836589635E-15</v>
+      </c>
+      <c r="AZ69">
+        <v>-14.24341029999999</v>
+      </c>
+      <c r="BA69">
+        <v>23.7079193</v>
+      </c>
+      <c r="BB69">
+        <v>0</v>
+      </c>
+      <c r="BC69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:20">
+    <row r="70" spans="1:55">
       <c r="A70" s="1">
         <v>69</v>
       </c>
-      <c r="B70">
-        <v>0</v>
+      <c r="B70" t="s">
+        <v>56</v>
       </c>
       <c r="C70" t="s">
         <v>57</v>
@@ -8868,13 +11202,16 @@
       <c r="T70">
         <v>0.03</v>
       </c>
+      <c r="X70" t="s">
+        <v>153</v>
+      </c>
     </row>
-    <row r="71" spans="1:20">
+    <row r="71" spans="1:55">
       <c r="A71" s="1">
         <v>70</v>
       </c>
-      <c r="B71">
-        <v>0</v>
+      <c r="B71" t="s">
+        <v>55</v>
       </c>
       <c r="C71" t="s">
         <v>57</v>
@@ -8924,13 +11261,112 @@
       <c r="R71" t="s">
         <v>82</v>
       </c>
+      <c r="U71">
+        <v>344.7823273104698</v>
+      </c>
+      <c r="V71">
+        <v>29.98958333333333</v>
+      </c>
+      <c r="W71">
+        <v>1753.388987599996</v>
+      </c>
+      <c r="X71" t="s">
+        <v>154</v>
+      </c>
+      <c r="Y71">
+        <v>344.7823273104698</v>
+      </c>
+      <c r="Z71">
+        <v>326.7823273104698</v>
+      </c>
+      <c r="AA71">
+        <v>18</v>
+      </c>
+      <c r="AB71">
+        <v>18</v>
+      </c>
+      <c r="AC71">
+        <v>438</v>
+      </c>
+      <c r="AD71">
+        <v>6.943021896517559</v>
+      </c>
+      <c r="AE71">
+        <v>0</v>
+      </c>
+      <c r="AF71">
+        <v>0</v>
+      </c>
+      <c r="AG71">
+        <v>0.1670675405657297</v>
+      </c>
+      <c r="AH71">
+        <v>0.1670675405657297</v>
+      </c>
+      <c r="AI71">
+        <v>0.1583454701694846</v>
+      </c>
+      <c r="AK71">
+        <v>106.6033800307256</v>
+      </c>
+      <c r="AL71">
+        <v>220.1789472797442</v>
+      </c>
+      <c r="AN71">
+        <v>58.68704411253908</v>
+      </c>
+      <c r="AO71">
+        <v>1514.038146022922</v>
+      </c>
+      <c r="AP71">
+        <v>549.6920444315269</v>
+      </c>
+      <c r="AQ71">
+        <v>2063.730190454449</v>
+      </c>
+      <c r="AR71">
+        <v>475.3545887162526</v>
+      </c>
+      <c r="AS71">
+        <v>1648.901323576857</v>
+      </c>
+      <c r="AT71">
+        <v>34.91296038251956</v>
+      </c>
+      <c r="AU71">
+        <v>224.8192448621507</v>
+      </c>
+      <c r="AV71">
+        <v>4.640297582406499</v>
+      </c>
+      <c r="AW71">
+        <v>177.6723000512094</v>
+      </c>
+      <c r="AX71">
+        <v>0</v>
+      </c>
+      <c r="AY71">
+        <v>0</v>
+      </c>
+      <c r="AZ71">
+        <v>-16.59457687080194</v>
+      </c>
+      <c r="BA71">
+        <v>11.74345269436844</v>
+      </c>
+      <c r="BB71">
+        <v>0</v>
+      </c>
+      <c r="BC71">
+        <v>0</v>
+      </c>
     </row>
-    <row r="72" spans="1:20">
+    <row r="72" spans="1:55">
       <c r="A72" s="1">
         <v>71</v>
       </c>
-      <c r="B72">
-        <v>0</v>
+      <c r="B72" t="s">
+        <v>55</v>
       </c>
       <c r="C72" t="s">
         <v>57</v>
@@ -8980,13 +11416,112 @@
       <c r="R72" t="s">
         <v>82</v>
       </c>
+      <c r="U72">
+        <v>347.7901518128196</v>
+      </c>
+      <c r="V72">
+        <v>29.98958333333333</v>
+      </c>
+      <c r="W72">
+        <v>1772.595983199993</v>
+      </c>
+      <c r="X72" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y72">
+        <v>347.7901518128196</v>
+      </c>
+      <c r="Z72">
+        <v>329.7901518128196</v>
+      </c>
+      <c r="AA72">
+        <v>18</v>
+      </c>
+      <c r="AB72">
+        <v>18</v>
+      </c>
+      <c r="AC72">
+        <v>438</v>
+      </c>
+      <c r="AD72">
+        <v>6.943021896517559</v>
+      </c>
+      <c r="AE72">
+        <v>0</v>
+      </c>
+      <c r="AF72">
+        <v>0</v>
+      </c>
+      <c r="AG72">
+        <v>0.1685250104017878</v>
+      </c>
+      <c r="AH72">
+        <v>0.1685250104017878</v>
+      </c>
+      <c r="AI72">
+        <v>0.1598029400055427</v>
+      </c>
+      <c r="AK72">
+        <v>109.10934</v>
+      </c>
+      <c r="AL72">
+        <v>220.6808118128196</v>
+      </c>
+      <c r="AN72">
+        <v>58.68704411253908</v>
+      </c>
+      <c r="AO72">
+        <v>1514.038146022922</v>
+      </c>
+      <c r="AP72">
+        <v>549.6920444315269</v>
+      </c>
+      <c r="AQ72">
+        <v>2063.730190454449</v>
+      </c>
+      <c r="AR72">
+        <v>475.3545887162526</v>
+      </c>
+      <c r="AS72">
+        <v>1636.982242316473</v>
+      </c>
+      <c r="AT72">
+        <v>22.9715242290566</v>
+      </c>
+      <c r="AU72">
+        <v>224.5054716243451</v>
+      </c>
+      <c r="AV72">
+        <v>3.824659811525552</v>
+      </c>
+      <c r="AW72">
+        <v>181.8489</v>
+      </c>
+      <c r="AX72">
+        <v>0</v>
+      </c>
+      <c r="AY72">
+        <v>0</v>
+      </c>
+      <c r="AZ72">
+        <v>-13.56230000000001</v>
+      </c>
+      <c r="BA72">
+        <v>12.9615</v>
+      </c>
+      <c r="BB72">
+        <v>0</v>
+      </c>
+      <c r="BC72">
+        <v>0</v>
+      </c>
     </row>
-    <row r="73" spans="1:20">
+    <row r="73" spans="1:55">
       <c r="A73" s="1">
         <v>72</v>
       </c>
-      <c r="B73">
-        <v>0</v>
+      <c r="B73" t="s">
+        <v>55</v>
       </c>
       <c r="C73" t="s">
         <v>57</v>
@@ -9035,6 +11570,105 @@
       </c>
       <c r="R73" t="s">
         <v>83</v>
+      </c>
+      <c r="U73">
+        <v>418.6846936943224</v>
+      </c>
+      <c r="V73">
+        <v>29.98958333333333</v>
+      </c>
+      <c r="W73">
+        <v>1312.511116499998</v>
+      </c>
+      <c r="X73" t="s">
+        <v>156</v>
+      </c>
+      <c r="Y73">
+        <v>418.6846936943224</v>
+      </c>
+      <c r="Z73">
+        <v>400.6846936943224</v>
+      </c>
+      <c r="AA73">
+        <v>18</v>
+      </c>
+      <c r="AB73">
+        <v>18</v>
+      </c>
+      <c r="AC73">
+        <v>438</v>
+      </c>
+      <c r="AD73">
+        <v>6.943021896517559</v>
+      </c>
+      <c r="AE73">
+        <v>0</v>
+      </c>
+      <c r="AF73">
+        <v>0</v>
+      </c>
+      <c r="AG73">
+        <v>0.2028776317906774</v>
+      </c>
+      <c r="AH73">
+        <v>0.2028776317906774</v>
+      </c>
+      <c r="AI73">
+        <v>0.1941555613944323</v>
+      </c>
+      <c r="AK73">
+        <v>121.1359295774175</v>
+      </c>
+      <c r="AL73">
+        <v>279.548764116905</v>
+      </c>
+      <c r="AN73">
+        <v>58.68704411253908</v>
+      </c>
+      <c r="AO73">
+        <v>1514.038146022922</v>
+      </c>
+      <c r="AP73">
+        <v>549.6920444315281</v>
+      </c>
+      <c r="AQ73">
+        <v>2063.73019045445</v>
+      </c>
+      <c r="AR73">
+        <v>475.3545887162526</v>
+      </c>
+      <c r="AS73">
+        <v>1590.590509650287</v>
+      </c>
+      <c r="AT73">
+        <v>3.304060741572887E-15</v>
+      </c>
+      <c r="AU73">
+        <v>279.548764116905</v>
+      </c>
+      <c r="AV73">
+        <v>2.502601113489304E-16</v>
+      </c>
+      <c r="AW73">
+        <v>201.8932159623624</v>
+      </c>
+      <c r="AX73">
+        <v>0</v>
+      </c>
+      <c r="AY73">
+        <v>0</v>
+      </c>
+      <c r="AZ73">
+        <v>0</v>
+      </c>
+      <c r="BA73">
+        <v>0</v>
+      </c>
+      <c r="BB73">
+        <v>0</v>
+      </c>
+      <c r="BC73">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>